<commit_message>
Product is being export to excel
</commit_message>
<xml_diff>
--- a/public/test.xlsx
+++ b/public/test.xlsx
@@ -15,9 +15,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
   <si>
     <t>Código</t>
+  </si>
+  <si>
+    <t>Nome</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t>Unidade</t>
+  </si>
+  <si>
+    <t>Marca</t>
+  </si>
+  <si>
+    <t>Grupo</t>
+  </si>
+  <si>
+    <t>s35</t>
+  </si>
+  <si>
+    <t>SORVETE NATA</t>
+  </si>
+  <si>
+    <t>SORVETE NATA (4X1,5L)</t>
+  </si>
+  <si>
+    <t>LPC- Sorv PT 1,5L NOBRE BCD</t>
+  </si>
+  <si>
+    <t>Caixa</t>
+  </si>
+  <si>
+    <t>Bariloche</t>
+  </si>
+  <si>
+    <t>Sorvete</t>
+  </si>
+  <si>
+    <t>S2626</t>
+  </si>
+  <si>
+    <t>SORVETE 1,5L MOUSSE LIMAO</t>
+  </si>
+  <si>
+    <t>SORVETE 1,5L MOUSSE LIMAO (4X1,5L)</t>
+  </si>
+  <si>
+    <t>LPC- Sorv PT 1,8L MESCLADO BCD</t>
+  </si>
+  <si>
+    <t>S262</t>
+  </si>
+  <si>
+    <t>SORVETE FRUTAS VERM</t>
+  </si>
+  <si>
+    <t>SORVETE FRUTAS VERM (4X1,5L)</t>
   </si>
 </sst>
 </file>
@@ -25,13 +85,22 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <b val="0"/>
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
@@ -53,8 +122,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -356,17 +428,113 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="8.712158" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="30.563965" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="41.132813" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="36.419678" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="9.997559" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="11.711426" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="9.283447" bestFit="true" customWidth="true" style="0"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>